<commit_message>
new: more informations about the dataset
</commit_message>
<xml_diff>
--- a/Tableau_regression_COX.xlsx
+++ b/Tableau_regression_COX.xlsx
@@ -52,7 +52,7 @@
     <t xml:space="preserve">&gt;90</t>
   </si>
   <si>
-    <t xml:space="preserve">Anéthésie</t>
+    <t xml:space="preserve">Anésthésie</t>
   </si>
   <si>
     <t xml:space="preserve">AG</t>
@@ -499,14 +499,14 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="6.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="6.57"/>

</xml_diff>